<commit_message>
creo tabella saldo del mese
</commit_message>
<xml_diff>
--- a/conti_camerino_styled.xlsx
+++ b/conti_camerino_styled.xlsx
@@ -112,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -164,6 +164,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -547,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2466,6 +2467,41 @@
       <c r="C158" s="8" t="inlineStr"/>
       <c r="D158" s="13" t="n">
         <v>106408.65</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2508,7 +2544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4425,6 +4461,41 @@
       <c r="C159" s="8" t="inlineStr"/>
       <c r="D159" s="13" t="n">
         <v>133297.72</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4466,7 +4537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6476,6 +6547,41 @@
       <c r="C165" s="8" t="inlineStr"/>
       <c r="D165" s="13" t="n">
         <v>98226.42</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -6517,7 +6623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8404,6 +8510,41 @@
       <c r="C155" s="8" t="inlineStr"/>
       <c r="D155" s="13" t="n">
         <v>151296.82</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -8447,7 +8588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10750,6 +10891,41 @@
       <c r="C184" s="8" t="inlineStr"/>
       <c r="D184" s="13" t="n">
         <v>144689.16</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -10794,7 +10970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12728,6 +12904,41 @@
       <c r="C160" s="8" t="inlineStr"/>
       <c r="D160" s="13" t="n">
         <v>125645.94</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -12770,7 +12981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14815,6 +15026,41 @@
       <c r="C164" s="8" t="inlineStr"/>
       <c r="D164" s="13" t="n">
         <v>133884.68</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -14861,7 +15107,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17088,6 +17334,41 @@
       <c r="C178" s="8" t="inlineStr"/>
       <c r="D178" s="13" t="n">
         <v>159744.75</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="B183" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -17132,7 +17413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D154"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19087,6 +19368,41 @@
       <c r="C154" s="8" t="inlineStr"/>
       <c r="D154" s="13" t="n">
         <v>116295.29</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -19131,7 +19447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21142,6 +21458,41 @@
       <c r="C165" s="8" t="inlineStr"/>
       <c r="D165" s="13" t="n">
         <v>105490.53</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -21184,7 +21535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22818,6 +23169,41 @@
       <c r="C136" s="8" t="inlineStr"/>
       <c r="D136" s="13" t="n">
         <v>62827.42</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -22858,7 +23244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24778,6 +25164,41 @@
       <c r="C156" s="8" t="inlineStr"/>
       <c r="D156" s="13" t="n">
         <v>95671.71000000001</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese precedente</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" s="19" t="inlineStr">
+        <is>
+          <t>ENTRATE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" s="19" t="inlineStr">
+        <is>
+          <t>USCITE del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" s="19" t="inlineStr">
+        <is>
+          <t>DIS/AVANZO del mese</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" s="19" t="inlineStr">
+        <is>
+          <t>SALDO del mese corrente</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saldo_ok_fino a gennaio compreso
</commit_message>
<xml_diff>
--- a/conti_camerino_styled.xlsx
+++ b/conti_camerino_styled.xlsx
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -179,6 +179,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2483,79 +2484,46 @@
         <v>106408.65</v>
       </c>
     </row>
-    <row r="159">
-      <c r="B159" s="14" t="n"/>
-      <c r="C159" s="15" t="n"/>
-      <c r="D159" s="9" t="n"/>
-    </row>
-    <row r="160">
-      <c r="B160" s="14" t="n"/>
-      <c r="C160" s="15" t="n"/>
-      <c r="D160" s="9" t="n"/>
-    </row>
-    <row r="161">
-      <c r="B161" s="14" t="n"/>
-      <c r="C161" s="15" t="n"/>
-      <c r="D161" s="9" t="n"/>
-    </row>
-    <row r="162">
-      <c r="B162" s="14" t="n"/>
-      <c r="C162" s="15" t="n"/>
-      <c r="D162" s="9" t="n"/>
-    </row>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
     <row r="163">
       <c r="B163" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C163" s="15" t="n"/>
-      <c r="D163" s="9" t="n"/>
-    </row>
-    <row r="164">
-      <c r="B164" s="14" t="n"/>
-      <c r="C164" s="15" t="n"/>
-      <c r="D164" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="164"/>
     <row r="165">
       <c r="B165" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C165" s="15" t="n"/>
       <c r="D165" s="20" t="n">
         <v>78144.25999999999</v>
       </c>
     </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
+    <row r="166"/>
     <row r="167">
       <c r="B167" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C167" s="15" t="n"/>
       <c r="D167" s="21" t="n">
         <v>106408.65</v>
       </c>
     </row>
-    <row r="168">
-      <c r="B168" s="14" t="n"/>
-      <c r="C168" s="15" t="n"/>
-      <c r="D168" s="9" t="n"/>
-    </row>
+    <row r="168"/>
     <row r="169">
       <c r="B169" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C169" s="15" t="n"/>
       <c r="D169" s="13" t="n">
         <v>-28264.39000000001</v>
       </c>
@@ -4527,79 +4495,46 @@
         <v>133297.72</v>
       </c>
     </row>
-    <row r="160">
-      <c r="B160" s="14" t="n"/>
-      <c r="C160" s="15" t="n"/>
-      <c r="D160" s="9" t="n"/>
-    </row>
-    <row r="161">
-      <c r="B161" s="14" t="n"/>
-      <c r="C161" s="15" t="n"/>
-      <c r="D161" s="9" t="n"/>
-    </row>
-    <row r="162">
-      <c r="B162" s="14" t="n"/>
-      <c r="C162" s="15" t="n"/>
-      <c r="D162" s="9" t="n"/>
-    </row>
-    <row r="163">
-      <c r="B163" s="14" t="n"/>
-      <c r="C163" s="15" t="n"/>
-      <c r="D163" s="9" t="n"/>
-    </row>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
     <row r="164">
       <c r="B164" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C164" s="15" t="n"/>
-      <c r="D164" s="9" t="n"/>
-    </row>
-    <row r="165">
-      <c r="B165" s="14" t="n"/>
-      <c r="C165" s="15" t="n"/>
-      <c r="D165" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="165"/>
     <row r="166">
       <c r="B166" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C166" s="15" t="n"/>
       <c r="D166" s="20" t="n">
         <v>97706.60000000001</v>
       </c>
     </row>
-    <row r="167">
-      <c r="B167" s="14" t="n"/>
-      <c r="C167" s="15" t="n"/>
-      <c r="D167" s="9" t="n"/>
-    </row>
+    <row r="167"/>
     <row r="168">
       <c r="B168" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C168" s="15" t="n"/>
       <c r="D168" s="21" t="n">
         <v>133297.72</v>
       </c>
     </row>
-    <row r="169">
-      <c r="B169" s="14" t="n"/>
-      <c r="C169" s="15" t="n"/>
-      <c r="D169" s="9" t="n"/>
-    </row>
+    <row r="169"/>
     <row r="170">
       <c r="B170" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C170" s="15" t="n"/>
       <c r="D170" s="13" t="n">
         <v>-35591.12</v>
       </c>
@@ -6663,79 +6598,46 @@
         <v>98226.42</v>
       </c>
     </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
-    <row r="167">
-      <c r="B167" s="14" t="n"/>
-      <c r="C167" s="15" t="n"/>
-      <c r="D167" s="9" t="n"/>
-    </row>
-    <row r="168">
-      <c r="B168" s="14" t="n"/>
-      <c r="C168" s="15" t="n"/>
-      <c r="D168" s="9" t="n"/>
-    </row>
-    <row r="169">
-      <c r="B169" s="14" t="n"/>
-      <c r="C169" s="15" t="n"/>
-      <c r="D169" s="9" t="n"/>
-    </row>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
     <row r="170">
       <c r="B170" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C170" s="15" t="n"/>
-      <c r="D170" s="9" t="n"/>
-    </row>
-    <row r="171">
-      <c r="B171" s="14" t="n"/>
-      <c r="C171" s="15" t="n"/>
-      <c r="D171" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="171"/>
     <row r="172">
       <c r="B172" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C172" s="15" t="n"/>
       <c r="D172" s="20" t="n">
         <v>70497.86</v>
       </c>
     </row>
-    <row r="173">
-      <c r="B173" s="14" t="n"/>
-      <c r="C173" s="15" t="n"/>
-      <c r="D173" s="9" t="n"/>
-    </row>
+    <row r="173"/>
     <row r="174">
       <c r="B174" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C174" s="15" t="n"/>
       <c r="D174" s="21" t="n">
         <v>98226.42000000001</v>
       </c>
     </row>
-    <row r="175">
-      <c r="B175" s="14" t="n"/>
-      <c r="C175" s="15" t="n"/>
-      <c r="D175" s="9" t="n"/>
-    </row>
+    <row r="175"/>
     <row r="176">
       <c r="B176" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C176" s="15" t="n"/>
       <c r="D176" s="13" t="n">
         <v>-27728.56000000001</v>
       </c>
@@ -8676,79 +8578,46 @@
         <v>151296.82</v>
       </c>
     </row>
-    <row r="156">
-      <c r="B156" s="14" t="n"/>
-      <c r="C156" s="15" t="n"/>
-      <c r="D156" s="9" t="n"/>
-    </row>
-    <row r="157">
-      <c r="B157" s="14" t="n"/>
-      <c r="C157" s="15" t="n"/>
-      <c r="D157" s="9" t="n"/>
-    </row>
-    <row r="158">
-      <c r="B158" s="14" t="n"/>
-      <c r="C158" s="15" t="n"/>
-      <c r="D158" s="9" t="n"/>
-    </row>
-    <row r="159">
-      <c r="B159" s="14" t="n"/>
-      <c r="C159" s="15" t="n"/>
-      <c r="D159" s="9" t="n"/>
-    </row>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
     <row r="160">
       <c r="B160" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C160" s="15" t="n"/>
-      <c r="D160" s="9" t="n"/>
-    </row>
-    <row r="161">
-      <c r="B161" s="14" t="n"/>
-      <c r="C161" s="15" t="n"/>
-      <c r="D161" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="161"/>
     <row r="162">
       <c r="B162" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C162" s="15" t="n"/>
       <c r="D162" s="20" t="n">
         <v>102393.39</v>
       </c>
     </row>
-    <row r="163">
-      <c r="B163" s="14" t="n"/>
-      <c r="C163" s="15" t="n"/>
-      <c r="D163" s="9" t="n"/>
-    </row>
+    <row r="163"/>
     <row r="164">
       <c r="B164" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C164" s="15" t="n"/>
       <c r="D164" s="21" t="n">
         <v>151296.82</v>
       </c>
     </row>
-    <row r="165">
-      <c r="B165" s="14" t="n"/>
-      <c r="C165" s="15" t="n"/>
-      <c r="D165" s="9" t="n"/>
-    </row>
+    <row r="165"/>
     <row r="166">
       <c r="B166" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C166" s="15" t="n"/>
       <c r="D166" s="13" t="n">
         <v>-48903.43000000001</v>
       </c>
@@ -11117,8 +10986,8 @@
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="D189" s="13" t="n">
-        <v>-100000</v>
+      <c r="D189" s="20" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="190"/>
@@ -11160,6 +11029,9 @@
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D197" s="22" t="n">
+        <v>57577.44399999999</v>
       </c>
     </row>
   </sheetData>
@@ -13140,79 +13012,46 @@
         <v>125645.94</v>
       </c>
     </row>
-    <row r="161">
-      <c r="B161" s="14" t="n"/>
-      <c r="C161" s="15" t="n"/>
-      <c r="D161" s="9" t="n"/>
-    </row>
-    <row r="162">
-      <c r="B162" s="14" t="n"/>
-      <c r="C162" s="15" t="n"/>
-      <c r="D162" s="9" t="n"/>
-    </row>
-    <row r="163">
-      <c r="B163" s="14" t="n"/>
-      <c r="C163" s="15" t="n"/>
-      <c r="D163" s="9" t="n"/>
-    </row>
-    <row r="164">
-      <c r="B164" s="14" t="n"/>
-      <c r="C164" s="15" t="n"/>
-      <c r="D164" s="9" t="n"/>
-    </row>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
     <row r="165">
       <c r="B165" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C165" s="15" t="n"/>
-      <c r="D165" s="9" t="n"/>
-    </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="166"/>
     <row r="167">
       <c r="B167" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C167" s="15" t="n"/>
       <c r="D167" s="20" t="n">
         <v>77543.88</v>
       </c>
     </row>
-    <row r="168">
-      <c r="B168" s="14" t="n"/>
-      <c r="C168" s="15" t="n"/>
-      <c r="D168" s="9" t="n"/>
-    </row>
+    <row r="168"/>
     <row r="169">
       <c r="B169" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C169" s="15" t="n"/>
       <c r="D169" s="21" t="n">
         <v>125645.94</v>
       </c>
     </row>
-    <row r="170">
-      <c r="B170" s="14" t="n"/>
-      <c r="C170" s="15" t="n"/>
-      <c r="D170" s="9" t="n"/>
-    </row>
+    <row r="170"/>
     <row r="171">
       <c r="B171" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C171" s="15" t="n"/>
       <c r="D171" s="13" t="n">
         <v>-48102.06</v>
       </c>
@@ -15312,79 +15151,46 @@
         <v>133884.68</v>
       </c>
     </row>
-    <row r="165">
-      <c r="B165" s="14" t="n"/>
-      <c r="C165" s="15" t="n"/>
-      <c r="D165" s="9" t="n"/>
-    </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
-    <row r="167">
-      <c r="B167" s="14" t="n"/>
-      <c r="C167" s="15" t="n"/>
-      <c r="D167" s="9" t="n"/>
-    </row>
-    <row r="168">
-      <c r="B168" s="14" t="n"/>
-      <c r="C168" s="15" t="n"/>
-      <c r="D168" s="9" t="n"/>
-    </row>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
     <row r="169">
       <c r="B169" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C169" s="15" t="n"/>
-      <c r="D169" s="9" t="n"/>
-    </row>
-    <row r="170">
-      <c r="B170" s="14" t="n"/>
-      <c r="C170" s="15" t="n"/>
-      <c r="D170" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="170"/>
     <row r="171">
       <c r="B171" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C171" s="15" t="n"/>
       <c r="D171" s="20" t="n">
         <v>77550.48999999999</v>
       </c>
     </row>
-    <row r="172">
-      <c r="B172" s="14" t="n"/>
-      <c r="C172" s="15" t="n"/>
-      <c r="D172" s="9" t="n"/>
-    </row>
+    <row r="172"/>
     <row r="173">
       <c r="B173" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C173" s="15" t="n"/>
       <c r="D173" s="21" t="n">
         <v>133884.68</v>
       </c>
     </row>
-    <row r="174">
-      <c r="B174" s="14" t="n"/>
-      <c r="C174" s="15" t="n"/>
-      <c r="D174" s="9" t="n"/>
-    </row>
+    <row r="174"/>
     <row r="175">
       <c r="B175" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C175" s="15" t="n"/>
       <c r="D175" s="13" t="n">
         <v>-56334.19</v>
       </c>
@@ -17670,79 +17476,46 @@
         <v>159744.75</v>
       </c>
     </row>
-    <row r="179">
-      <c r="B179" s="14" t="n"/>
-      <c r="C179" s="15" t="n"/>
-      <c r="D179" s="9" t="n"/>
-    </row>
-    <row r="180">
-      <c r="B180" s="14" t="n"/>
-      <c r="C180" s="15" t="n"/>
-      <c r="D180" s="9" t="n"/>
-    </row>
-    <row r="181">
-      <c r="B181" s="14" t="n"/>
-      <c r="C181" s="15" t="n"/>
-      <c r="D181" s="9" t="n"/>
-    </row>
-    <row r="182">
-      <c r="B182" s="14" t="n"/>
-      <c r="C182" s="15" t="n"/>
-      <c r="D182" s="9" t="n"/>
-    </row>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
     <row r="183">
       <c r="B183" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C183" s="15" t="n"/>
-      <c r="D183" s="9" t="n"/>
-    </row>
-    <row r="184">
-      <c r="B184" s="14" t="n"/>
-      <c r="C184" s="15" t="n"/>
-      <c r="D184" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="184"/>
     <row r="185">
       <c r="B185" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C185" s="15" t="n"/>
       <c r="D185" s="20" t="n">
         <v>100705.39</v>
       </c>
     </row>
-    <row r="186">
-      <c r="B186" s="14" t="n"/>
-      <c r="C186" s="15" t="n"/>
-      <c r="D186" s="9" t="n"/>
-    </row>
+    <row r="186"/>
     <row r="187">
       <c r="B187" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C187" s="15" t="n"/>
       <c r="D187" s="21" t="n">
         <v>159744.75</v>
       </c>
     </row>
-    <row r="188">
-      <c r="B188" s="14" t="n"/>
-      <c r="C188" s="15" t="n"/>
-      <c r="D188" s="9" t="n"/>
-    </row>
+    <row r="188"/>
     <row r="189">
       <c r="B189" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C189" s="15" t="n"/>
       <c r="D189" s="13" t="n">
         <v>-59039.36</v>
       </c>
@@ -19754,79 +19527,46 @@
         <v>116295.29</v>
       </c>
     </row>
-    <row r="155">
-      <c r="B155" s="14" t="n"/>
-      <c r="C155" s="15" t="n"/>
-      <c r="D155" s="9" t="n"/>
-    </row>
-    <row r="156">
-      <c r="B156" s="14" t="n"/>
-      <c r="C156" s="15" t="n"/>
-      <c r="D156" s="9" t="n"/>
-    </row>
-    <row r="157">
-      <c r="B157" s="14" t="n"/>
-      <c r="C157" s="15" t="n"/>
-      <c r="D157" s="9" t="n"/>
-    </row>
-    <row r="158">
-      <c r="B158" s="14" t="n"/>
-      <c r="C158" s="15" t="n"/>
-      <c r="D158" s="9" t="n"/>
-    </row>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
     <row r="159">
       <c r="B159" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C159" s="15" t="n"/>
-      <c r="D159" s="9" t="n"/>
-    </row>
-    <row r="160">
-      <c r="B160" s="14" t="n"/>
-      <c r="C160" s="15" t="n"/>
-      <c r="D160" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="160"/>
     <row r="161">
       <c r="B161" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C161" s="15" t="n"/>
       <c r="D161" s="20" t="n">
         <v>107413.59</v>
       </c>
     </row>
-    <row r="162">
-      <c r="B162" s="14" t="n"/>
-      <c r="C162" s="15" t="n"/>
-      <c r="D162" s="9" t="n"/>
-    </row>
+    <row r="162"/>
     <row r="163">
       <c r="B163" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C163" s="15" t="n"/>
       <c r="D163" s="21" t="n">
         <v>116295.29</v>
       </c>
     </row>
-    <row r="164">
-      <c r="B164" s="14" t="n"/>
-      <c r="C164" s="15" t="n"/>
-      <c r="D164" s="9" t="n"/>
-    </row>
+    <row r="164"/>
     <row r="165">
       <c r="B165" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C165" s="15" t="n"/>
       <c r="D165" s="13" t="n">
         <v>-8881.700000000012</v>
       </c>
@@ -21894,79 +21634,46 @@
         <v>105490.53</v>
       </c>
     </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
-    <row r="167">
-      <c r="B167" s="14" t="n"/>
-      <c r="C167" s="15" t="n"/>
-      <c r="D167" s="9" t="n"/>
-    </row>
-    <row r="168">
-      <c r="B168" s="14" t="n"/>
-      <c r="C168" s="15" t="n"/>
-      <c r="D168" s="9" t="n"/>
-    </row>
-    <row r="169">
-      <c r="B169" s="14" t="n"/>
-      <c r="C169" s="15" t="n"/>
-      <c r="D169" s="9" t="n"/>
-    </row>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
     <row r="170">
       <c r="B170" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C170" s="15" t="n"/>
-      <c r="D170" s="9" t="n"/>
-    </row>
-    <row r="171">
-      <c r="B171" s="14" t="n"/>
-      <c r="C171" s="15" t="n"/>
-      <c r="D171" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="171"/>
     <row r="172">
       <c r="B172" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C172" s="15" t="n"/>
       <c r="D172" s="20" t="n">
         <v>58442.47</v>
       </c>
     </row>
-    <row r="173">
-      <c r="B173" s="14" t="n"/>
-      <c r="C173" s="15" t="n"/>
-      <c r="D173" s="9" t="n"/>
-    </row>
+    <row r="173"/>
     <row r="174">
       <c r="B174" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C174" s="15" t="n"/>
       <c r="D174" s="21" t="n">
         <v>105490.53</v>
       </c>
     </row>
-    <row r="175">
-      <c r="B175" s="14" t="n"/>
-      <c r="C175" s="15" t="n"/>
-      <c r="D175" s="9" t="n"/>
-    </row>
+    <row r="175"/>
     <row r="176">
       <c r="B176" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C176" s="15" t="n"/>
       <c r="D176" s="13" t="n">
         <v>-47048.06</v>
       </c>
@@ -23655,79 +23362,46 @@
         <v>62827.42</v>
       </c>
     </row>
-    <row r="137">
-      <c r="B137" s="14" t="n"/>
-      <c r="C137" s="15" t="n"/>
-      <c r="D137" s="9" t="n"/>
-    </row>
-    <row r="138">
-      <c r="B138" s="14" t="n"/>
-      <c r="C138" s="15" t="n"/>
-      <c r="D138" s="9" t="n"/>
-    </row>
-    <row r="139">
-      <c r="B139" s="14" t="n"/>
-      <c r="C139" s="15" t="n"/>
-      <c r="D139" s="9" t="n"/>
-    </row>
-    <row r="140">
-      <c r="B140" s="14" t="n"/>
-      <c r="C140" s="15" t="n"/>
-      <c r="D140" s="9" t="n"/>
-    </row>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
     <row r="141">
       <c r="B141" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C141" s="15" t="n"/>
-      <c r="D141" s="9" t="n"/>
-    </row>
-    <row r="142">
-      <c r="B142" s="14" t="n"/>
-      <c r="C142" s="15" t="n"/>
-      <c r="D142" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="142"/>
     <row r="143">
       <c r="B143" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C143" s="15" t="n"/>
       <c r="D143" s="20" t="n">
         <v>59532.41</v>
       </c>
     </row>
-    <row r="144">
-      <c r="B144" s="14" t="n"/>
-      <c r="C144" s="15" t="n"/>
-      <c r="D144" s="9" t="n"/>
-    </row>
+    <row r="144"/>
     <row r="145">
       <c r="B145" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C145" s="15" t="n"/>
       <c r="D145" s="21" t="n">
         <v>62827.42</v>
       </c>
     </row>
-    <row r="146">
-      <c r="B146" s="14" t="n"/>
-      <c r="C146" s="15" t="n"/>
-      <c r="D146" s="9" t="n"/>
-    </row>
+    <row r="146"/>
     <row r="147">
       <c r="B147" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C147" s="15" t="n"/>
       <c r="D147" s="13" t="n">
         <v>-3295.009999999995</v>
       </c>
@@ -25700,79 +25374,46 @@
         <v>95671.71000000001</v>
       </c>
     </row>
-    <row r="157">
-      <c r="B157" s="14" t="n"/>
-      <c r="C157" s="15" t="n"/>
-      <c r="D157" s="9" t="n"/>
-    </row>
-    <row r="158">
-      <c r="B158" s="14" t="n"/>
-      <c r="C158" s="15" t="n"/>
-      <c r="D158" s="9" t="n"/>
-    </row>
-    <row r="159">
-      <c r="B159" s="14" t="n"/>
-      <c r="C159" s="15" t="n"/>
-      <c r="D159" s="9" t="n"/>
-    </row>
-    <row r="160">
-      <c r="B160" s="14" t="n"/>
-      <c r="C160" s="15" t="n"/>
-      <c r="D160" s="9" t="n"/>
-    </row>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
     <row r="161">
       <c r="B161" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-      <c r="C161" s="15" t="n"/>
-      <c r="D161" s="9" t="n"/>
-    </row>
-    <row r="162">
-      <c r="B162" s="14" t="n"/>
-      <c r="C162" s="15" t="n"/>
-      <c r="D162" s="9" t="n"/>
-    </row>
+    </row>
+    <row r="162"/>
     <row r="163">
       <c r="B163" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-      <c r="C163" s="15" t="n"/>
       <c r="D163" s="20" t="n">
         <v>66470.95</v>
       </c>
     </row>
-    <row r="164">
-      <c r="B164" s="14" t="n"/>
-      <c r="C164" s="15" t="n"/>
-      <c r="D164" s="9" t="n"/>
-    </row>
+    <row r="164"/>
     <row r="165">
       <c r="B165" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-      <c r="C165" s="15" t="n"/>
       <c r="D165" s="21" t="n">
         <v>95671.71000000002</v>
       </c>
     </row>
-    <row r="166">
-      <c r="B166" s="14" t="n"/>
-      <c r="C166" s="15" t="n"/>
-      <c r="D166" s="9" t="n"/>
-    </row>
+    <row r="166"/>
     <row r="167">
       <c r="B167" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-      <c r="C167" s="15" t="n"/>
       <c r="D167" s="13" t="n">
         <v>-29200.76000000002</v>
       </c>

</xml_diff>

<commit_message>
conti_camerino_03_subtotal e saldo _ok
</commit_message>
<xml_diff>
--- a/conti_camerino_styled.xlsx
+++ b/conti_camerino_styled.xlsx
@@ -28,11 +28,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00€"/>
     <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+    <numFmt numFmtId="166" formatCode="-#,##0.00€"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,6 +78,10 @@
     <font>
       <b val="1"/>
       <color rgb="00000000"/>
+      <sz val="15"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="15"/>
     </font>
   </fonts>
@@ -141,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -195,6 +200,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2824,47 +2838,54 @@
         <v>353.3</v>
       </c>
     </row>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
     <row r="186">
       <c r="B186" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="187"/>
+      <c r="D186" s="22" t="n">
+        <v>-139380.4480000001</v>
+      </c>
+    </row>
     <row r="188">
       <c r="B188" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="189"/>
+      <c r="D188" s="20" t="n">
+        <v>78144.25999999999</v>
+      </c>
+    </row>
     <row r="190">
       <c r="B190" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="191"/>
+      <c r="D190" s="21" t="n">
+        <v>106408.65</v>
+      </c>
+    </row>
     <row r="192">
       <c r="B192" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="193"/>
+      <c r="D192" s="22" t="n">
+        <v>-28264.39000000001</v>
+      </c>
+    </row>
     <row r="194">
       <c r="B194" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D194" s="22" t="n">
+        <v>-181803.0040000001</v>
       </c>
     </row>
   </sheetData>
@@ -5145,47 +5166,54 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
     <row r="185">
       <c r="B185" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="186"/>
+      <c r="D185" s="22" t="n">
+        <v>-181803.0040000001</v>
+      </c>
+    </row>
     <row r="187">
       <c r="B187" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="188"/>
+      <c r="D187" s="20" t="n">
+        <v>97706.60000000001</v>
+      </c>
+    </row>
     <row r="189">
       <c r="B189" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="190"/>
+      <c r="D189" s="21" t="n">
+        <v>133297.72</v>
+      </c>
+    </row>
     <row r="191">
       <c r="B191" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="192"/>
+      <c r="D191" s="22" t="n">
+        <v>-35591.12</v>
+      </c>
+    </row>
     <row r="193">
       <c r="B193" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D193" s="22" t="n">
+        <v>-224225.5600000001</v>
       </c>
     </row>
   </sheetData>
@@ -7574,47 +7602,54 @@
         <v>1049.05</v>
       </c>
     </row>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
     <row r="194">
       <c r="B194" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="195"/>
+      <c r="D194" s="22" t="n">
+        <v>-224225.5600000001</v>
+      </c>
+    </row>
     <row r="196">
       <c r="B196" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="197"/>
+      <c r="D196" s="20" t="n">
+        <v>70497.86</v>
+      </c>
+    </row>
     <row r="198">
       <c r="B198" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="199"/>
+      <c r="D198" s="21" t="n">
+        <v>98226.42000000001</v>
+      </c>
+    </row>
     <row r="200">
       <c r="B200" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="201"/>
+      <c r="D200" s="22" t="n">
+        <v>-27728.56000000001</v>
+      </c>
+    </row>
     <row r="202">
       <c r="B202" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D202" s="22" t="n">
+        <v>-266648.1160000002</v>
       </c>
     </row>
   </sheetData>
@@ -9887,47 +9922,54 @@
         <v>115</v>
       </c>
     </row>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
     <row r="184">
       <c r="B184" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="185"/>
+      <c r="D184" s="22" t="n">
+        <v>-266648.1160000002</v>
+      </c>
+    </row>
     <row r="186">
       <c r="B186" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="187"/>
+      <c r="D186" s="20" t="n">
+        <v>102393.39</v>
+      </c>
+    </row>
     <row r="188">
       <c r="B188" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="189"/>
+      <c r="D188" s="21" t="n">
+        <v>151296.82</v>
+      </c>
+    </row>
     <row r="190">
       <c r="B190" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="191"/>
+      <c r="D190" s="22" t="n">
+        <v>-48903.43000000001</v>
+      </c>
+    </row>
     <row r="192">
       <c r="B192" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D192" s="22" t="n">
+        <v>-309070.6720000001</v>
       </c>
     </row>
   </sheetData>
@@ -12693,47 +12735,54 @@
         <v>262.32</v>
       </c>
     </row>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
     <row r="224">
       <c r="B224" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="225"/>
+      <c r="D224" s="20" t="n">
+        <v>200000</v>
+      </c>
+    </row>
     <row r="226">
       <c r="B226" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="227"/>
+      <c r="D226" s="20" t="n">
+        <v>102266.604</v>
+      </c>
+    </row>
     <row r="228">
       <c r="B228" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="229"/>
+      <c r="D228" s="21" t="n">
+        <v>144689.16</v>
+      </c>
+    </row>
     <row r="230">
       <c r="B230" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="231"/>
+      <c r="D230" s="22" t="n">
+        <v>-42422.55600000001</v>
+      </c>
+    </row>
     <row r="232">
       <c r="B232" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D232" s="20" t="n">
+        <v>157577.444</v>
       </c>
     </row>
   </sheetData>
@@ -15066,47 +15115,54 @@
         <v>896.83</v>
       </c>
     </row>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
     <row r="188">
       <c r="B188" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="189"/>
+      <c r="D188" s="20" t="n">
+        <v>157577.444</v>
+      </c>
+    </row>
     <row r="190">
       <c r="B190" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="191"/>
+      <c r="D190" s="20" t="n">
+        <v>77543.88</v>
+      </c>
+    </row>
     <row r="192">
       <c r="B192" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="193"/>
+      <c r="D192" s="21" t="n">
+        <v>125645.94</v>
+      </c>
+    </row>
     <row r="194">
       <c r="B194" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="195"/>
+      <c r="D194" s="22" t="n">
+        <v>-48102.06</v>
+      </c>
+    </row>
     <row r="196">
       <c r="B196" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D196" s="20" t="n">
+        <v>115154.888</v>
       </c>
     </row>
   </sheetData>
@@ -17594,47 +17650,54 @@
         <v>700</v>
       </c>
     </row>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
     <row r="201">
       <c r="B201" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="202"/>
+      <c r="D201" s="20" t="n">
+        <v>115154.888</v>
+      </c>
+    </row>
     <row r="203">
       <c r="B203" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="204"/>
+      <c r="D203" s="20" t="n">
+        <v>77550.48999999999</v>
+      </c>
+    </row>
     <row r="205">
       <c r="B205" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="206"/>
+      <c r="D205" s="21" t="n">
+        <v>133884.68</v>
+      </c>
+    </row>
     <row r="207">
       <c r="B207" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="208"/>
+      <c r="D207" s="22" t="n">
+        <v>-56334.19</v>
+      </c>
+    </row>
     <row r="209">
       <c r="B209" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D209" s="20" t="n">
+        <v>72732.33199999997</v>
       </c>
     </row>
   </sheetData>
@@ -20314,47 +20377,54 @@
         <v>325.73</v>
       </c>
     </row>
-    <row r="213"/>
-    <row r="214"/>
-    <row r="215"/>
-    <row r="216"/>
     <row r="217">
       <c r="B217" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="218"/>
+      <c r="D217" s="20" t="n">
+        <v>72732.33199999997</v>
+      </c>
+    </row>
     <row r="219">
       <c r="B219" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="220"/>
+      <c r="D219" s="20" t="n">
+        <v>100705.39</v>
+      </c>
+    </row>
     <row r="221">
       <c r="B221" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="222"/>
+      <c r="D221" s="21" t="n">
+        <v>159744.75</v>
+      </c>
+    </row>
     <row r="223">
       <c r="B223" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="224"/>
+      <c r="D223" s="22" t="n">
+        <v>-59039.36</v>
+      </c>
+    </row>
     <row r="225">
       <c r="B225" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D225" s="20" t="n">
+        <v>30309.77599999995</v>
       </c>
     </row>
   </sheetData>
@@ -22758,47 +22828,54 @@
         <v>1184.04</v>
       </c>
     </row>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
     <row r="195">
       <c r="B195" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="196"/>
+      <c r="D195" s="20" t="n">
+        <v>30309.77599999995</v>
+      </c>
+    </row>
     <row r="197">
       <c r="B197" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="198"/>
+      <c r="D197" s="20" t="n">
+        <v>107413.59</v>
+      </c>
+    </row>
     <row r="199">
       <c r="B199" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="200"/>
+      <c r="D199" s="21" t="n">
+        <v>116295.29</v>
+      </c>
+    </row>
     <row r="201">
       <c r="B201" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="202"/>
+      <c r="D201" s="22" t="n">
+        <v>-8881.700000000012</v>
+      </c>
+    </row>
     <row r="203">
       <c r="B203" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D203" s="22" t="n">
+        <v>-12112.78000000006</v>
       </c>
     </row>
   </sheetData>
@@ -25207,47 +25284,54 @@
         <v>1511.45</v>
       </c>
     </row>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
     <row r="195">
       <c r="B195" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="196"/>
+      <c r="D195" s="22" t="n">
+        <v>-12112.78000000006</v>
+      </c>
+    </row>
     <row r="197">
       <c r="B197" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="198"/>
+      <c r="D197" s="20" t="n">
+        <v>58442.47</v>
+      </c>
+    </row>
     <row r="199">
       <c r="B199" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="200"/>
+      <c r="D199" s="21" t="n">
+        <v>105490.53</v>
+      </c>
+    </row>
     <row r="201">
       <c r="B201" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="202"/>
+      <c r="D201" s="22" t="n">
+        <v>-47048.06</v>
+      </c>
+    </row>
     <row r="203">
       <c r="B203" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D203" s="22" t="n">
+        <v>-54535.33600000007</v>
       </c>
     </row>
   </sheetData>
@@ -27242,47 +27326,54 @@
         <v>1107.43</v>
       </c>
     </row>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
     <row r="161">
       <c r="B161" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="162"/>
+      <c r="D161" s="22" t="n">
+        <v>-54535.33600000007</v>
+      </c>
+    </row>
     <row r="163">
       <c r="B163" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="164"/>
+      <c r="D163" s="20" t="n">
+        <v>59532.41</v>
+      </c>
+    </row>
     <row r="165">
       <c r="B165" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="166"/>
+      <c r="D165" s="21" t="n">
+        <v>62827.42</v>
+      </c>
+    </row>
     <row r="167">
       <c r="B167" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="168"/>
+      <c r="D167" s="22" t="n">
+        <v>-3295.009999999995</v>
+      </c>
+    </row>
     <row r="169">
       <c r="B169" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D169" s="22" t="n">
+        <v>-96957.89200000008</v>
       </c>
     </row>
   </sheetData>
@@ -29603,47 +29694,54 @@
         <v>700</v>
       </c>
     </row>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
     <row r="188">
       <c r="B188" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese precedente</t>
         </is>
       </c>
-    </row>
-    <row r="189"/>
+      <c r="D188" s="22" t="n">
+        <v>-96957.89200000008</v>
+      </c>
+    </row>
     <row r="190">
       <c r="B190" s="19" t="inlineStr">
         <is>
           <t>ENTRATE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="191"/>
+      <c r="D190" s="20" t="n">
+        <v>66470.95</v>
+      </c>
+    </row>
     <row r="192">
       <c r="B192" s="19" t="inlineStr">
         <is>
           <t>USCITE del mese</t>
         </is>
       </c>
-    </row>
-    <row r="193"/>
+      <c r="D192" s="21" t="n">
+        <v>95671.71000000002</v>
+      </c>
+    </row>
     <row r="194">
       <c r="B194" s="19" t="inlineStr">
         <is>
           <t>DIS/AVANZO del mese</t>
         </is>
       </c>
-    </row>
-    <row r="195"/>
+      <c r="D194" s="22" t="n">
+        <v>-29200.76000000002</v>
+      </c>
+    </row>
     <row r="196">
       <c r="B196" s="19" t="inlineStr">
         <is>
           <t>SALDO del mese corrente</t>
         </is>
+      </c>
+      <c r="D196" s="22" t="n">
+        <v>-139380.4480000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conti_camerino_05 entrate_uscite in giallo
</commit_message>
<xml_diff>
--- a/conti_camerino_styled.xlsx
+++ b/conti_camerino_styled.xlsx
@@ -104,12 +104,17 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00d1d22e"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -174,7 +179,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">

</xml_diff>

<commit_message>
conti_camerino_07 tabellone_ landscape e pivot
</commit_message>
<xml_diff>
--- a/conti_camerino_styled.xlsx
+++ b/conti_camerino_styled.xlsx
@@ -139,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -188,11 +188,29 @@
         <color rgb="004617F1"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -263,6 +281,9 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -283,8 +304,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Pandas" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -10247,7 +10269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10256,10 +10278,729 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>Tabellone Entrate</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="26" t="n"/>
+      <c r="B2" s="26" t="inlineStr">
+        <is>
+          <t>gennaio</t>
+        </is>
+      </c>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>febbraio</t>
+        </is>
+      </c>
+      <c r="D2" s="26" t="inlineStr">
+        <is>
+          <t>marzo</t>
+        </is>
+      </c>
+      <c r="E2" s="26" t="inlineStr">
+        <is>
+          <t>aprile</t>
+        </is>
+      </c>
+      <c r="F2" s="26" t="inlineStr">
+        <is>
+          <t>maggio</t>
+        </is>
+      </c>
+      <c r="G2" s="26" t="inlineStr">
+        <is>
+          <t>giugno</t>
+        </is>
+      </c>
+      <c r="H2" s="26" t="inlineStr">
+        <is>
+          <t>luglio</t>
+        </is>
+      </c>
+      <c r="I2" s="26" t="inlineStr">
+        <is>
+          <t>agosto</t>
+        </is>
+      </c>
+      <c r="J2" s="26" t="inlineStr">
+        <is>
+          <t>settembre</t>
+        </is>
+      </c>
+      <c r="K2" s="26" t="inlineStr">
+        <is>
+          <t>ottobre</t>
+        </is>
+      </c>
+      <c r="L2" s="26" t="inlineStr">
+        <is>
+          <t>novembre</t>
+        </is>
+      </c>
+      <c r="M2" s="26" t="inlineStr">
+        <is>
+          <t>dicembre</t>
+        </is>
+      </c>
+      <c r="N2" s="26" t="inlineStr">
+        <is>
+          <t>TOTALE_Entrate</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="26" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="26" t="inlineStr">
+        <is>
+          <t>Collette-Chiesa</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4066.05</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4247.3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5041.3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5839.45</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3841.96</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2391.44</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3400.13</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4365.17</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3990.58</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3392.04</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2414.51</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3086.29</v>
+      </c>
+      <c r="N4" t="n">
+        <v>46076.22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="26" t="inlineStr">
+        <is>
+          <t>Congrua</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8676.85</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6768.86</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9714.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9460.09</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9566.23</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5483.1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>8603.93</v>
+      </c>
+      <c r="N5" t="n">
+        <v>85688.66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="26" t="inlineStr">
+        <is>
+          <t>Eccedenza Cassa</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1737.78</v>
+      </c>
+      <c r="C6" t="n">
+        <v>191.63</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>321.02</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2250.43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="26" t="inlineStr">
+        <is>
+          <t>Interessi</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>171.96</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>60.65</v>
+      </c>
+      <c r="E7" t="n">
+        <v>272.7</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>39.42</v>
+      </c>
+      <c r="H7" t="n">
+        <v>54.98</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>629.71</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="inlineStr">
+        <is>
+          <t>Messe celebrate</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10780</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9550</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10930</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10580</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11270</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10870</v>
+      </c>
+      <c r="H8" t="n">
+        <v>11640</v>
+      </c>
+      <c r="I8" t="n">
+        <v>11880</v>
+      </c>
+      <c r="J8" t="n">
+        <v>12140</v>
+      </c>
+      <c r="K8" t="n">
+        <v>12040</v>
+      </c>
+      <c r="L8" t="n">
+        <v>11170</v>
+      </c>
+      <c r="M8" t="n">
+        <v>11290</v>
+      </c>
+      <c r="N8" t="n">
+        <v>134140</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="26" t="inlineStr">
+        <is>
+          <t>Offerte</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>35640.7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15126</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17658.82</v>
+      </c>
+      <c r="E9" t="n">
+        <v>30682.97</v>
+      </c>
+      <c r="F9" t="n">
+        <v>38756.93</v>
+      </c>
+      <c r="G9" t="n">
+        <v>13729</v>
+      </c>
+      <c r="H9" t="n">
+        <v>18322</v>
+      </c>
+      <c r="I9" t="n">
+        <v>13447</v>
+      </c>
+      <c r="J9" t="n">
+        <v>20839.11</v>
+      </c>
+      <c r="K9" t="n">
+        <v>47738</v>
+      </c>
+      <c r="L9" t="n">
+        <v>15892</v>
+      </c>
+      <c r="M9" t="n">
+        <v>24622.91</v>
+      </c>
+      <c r="N9" t="n">
+        <v>292455.44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="26" t="inlineStr">
+        <is>
+          <t>Pensioni</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>19034</v>
+      </c>
+      <c r="C10" t="n">
+        <v>17399</v>
+      </c>
+      <c r="D10" t="n">
+        <v>16883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>16889</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17084</v>
+      </c>
+      <c r="G10" t="n">
+        <v>14530</v>
+      </c>
+      <c r="H10" t="n">
+        <v>11975</v>
+      </c>
+      <c r="I10" t="n">
+        <v>12148</v>
+      </c>
+      <c r="J10" t="n">
+        <v>12746</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12747</v>
+      </c>
+      <c r="L10" t="n">
+        <v>12748</v>
+      </c>
+      <c r="M10" t="n">
+        <v>24322</v>
+      </c>
+      <c r="N10" t="n">
+        <v>188505</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="26" t="inlineStr">
+        <is>
+          <t>Predicazione</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>150</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1020</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3340</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1090</v>
+      </c>
+      <c r="H11" t="n">
+        <v>280</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4090</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2250</v>
+      </c>
+      <c r="K11" t="n">
+        <v>660</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1780</v>
+      </c>
+      <c r="M11" t="n">
+        <v>270</v>
+      </c>
+      <c r="N11" t="n">
+        <v>15080</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="26" t="inlineStr">
+        <is>
+          <t>Salute</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2965.8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2167.61</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2041.91</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2328.89</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3318.57</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1451.49</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1394.77</v>
+      </c>
+      <c r="I12" t="n">
+        <v>453.99</v>
+      </c>
+      <c r="J12" t="n">
+        <v>900.5700000000001</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1546.76</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1809.17</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1447.61</v>
+      </c>
+      <c r="N12" t="n">
+        <v>21827.14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="26" t="inlineStr">
+        <is>
+          <t>Servizi religiosi</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6083</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4050</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5050</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8746</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8815</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3950</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2775</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3650</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3890</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4530</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5509</v>
+      </c>
+      <c r="M13" t="n">
+        <v>7374</v>
+      </c>
+      <c r="N13" t="n">
+        <v>64422</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="26" t="inlineStr">
+        <is>
+          <t>Stipendi</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2843.7</v>
+      </c>
+      <c r="D14" t="n">
+        <v>953.9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1095</v>
+      </c>
+      <c r="F14" t="n">
+        <v>950.9</v>
+      </c>
+      <c r="G14" t="n">
+        <v>950</v>
+      </c>
+      <c r="H14" t="n">
+        <v>950</v>
+      </c>
+      <c r="I14" t="n">
+        <v>950</v>
+      </c>
+      <c r="J14" t="n">
+        <v>950</v>
+      </c>
+      <c r="K14" t="n">
+        <v>950</v>
+      </c>
+      <c r="L14" t="n">
+        <v>950</v>
+      </c>
+      <c r="M14" t="n">
+        <v>950</v>
+      </c>
+      <c r="N14" t="n">
+        <v>12493.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="26" t="inlineStr">
+        <is>
+          <t>Sussidi</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>784.96</v>
+      </c>
+      <c r="C15" t="n">
+        <v>747.78</v>
+      </c>
+      <c r="D15" t="n">
+        <v>590.91</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1037.4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5963.2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>600</v>
+      </c>
+      <c r="H15" t="n">
+        <v>160.83</v>
+      </c>
+      <c r="I15" t="n">
+        <v>442.39</v>
+      </c>
+      <c r="J15" t="n">
+        <v>195</v>
+      </c>
+      <c r="K15" t="n">
+        <v>755</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1585.84</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2423.65</v>
+      </c>
+      <c r="N15" t="n">
+        <v>15286.96</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="26" t="inlineStr">
+        <is>
+          <t>Vendite varie</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>12175.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14422</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8475.9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12753.89</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4506.8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3037</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3096.6</v>
+      </c>
+      <c r="I16" t="n">
+        <v>9561.299999999999</v>
+      </c>
+      <c r="J16" t="n">
+        <v>14759.9</v>
+      </c>
+      <c r="K16" t="n">
+        <v>7864.7</v>
+      </c>
+      <c r="L16" t="n">
+        <v>11156.24</v>
+      </c>
+      <c r="M16" t="n">
+        <v>18003</v>
+      </c>
+      <c r="N16" t="n">
+        <v>119812.83</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="26" t="inlineStr">
+        <is>
+          <t>TOTALE_Entrate</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>102266.6</v>
+      </c>
+      <c r="C17" t="n">
+        <v>77543.88</v>
+      </c>
+      <c r="D17" t="n">
+        <v>77550.49000000001</v>
+      </c>
+      <c r="E17" t="n">
+        <v>100705.39</v>
+      </c>
+      <c r="F17" t="n">
+        <v>107413.59</v>
+      </c>
+      <c r="G17" t="n">
+        <v>58442.47</v>
+      </c>
+      <c r="H17" t="n">
+        <v>59532.41</v>
+      </c>
+      <c r="I17" t="n">
+        <v>66470.95</v>
+      </c>
+      <c r="J17" t="n">
+        <v>78144.25999999999</v>
+      </c>
+      <c r="K17" t="n">
+        <v>97706.60000000001</v>
+      </c>
+      <c r="L17" t="n">
+        <v>70497.86</v>
+      </c>
+      <c r="M17" t="n">
+        <v>102393.39</v>
+      </c>
+      <c r="N17" t="n">
+        <v>998667.89</v>
       </c>
     </row>
   </sheetData>
@@ -10274,7 +11015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10283,10 +11024,1097 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>Tabellone Uscite</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="26" t="n"/>
+      <c r="B2" s="26" t="inlineStr">
+        <is>
+          <t>gennaio</t>
+        </is>
+      </c>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>febbraio</t>
+        </is>
+      </c>
+      <c r="D2" s="26" t="inlineStr">
+        <is>
+          <t>marzo</t>
+        </is>
+      </c>
+      <c r="E2" s="26" t="inlineStr">
+        <is>
+          <t>aprile</t>
+        </is>
+      </c>
+      <c r="F2" s="26" t="inlineStr">
+        <is>
+          <t>maggio</t>
+        </is>
+      </c>
+      <c r="G2" s="26" t="inlineStr">
+        <is>
+          <t>giugno</t>
+        </is>
+      </c>
+      <c r="H2" s="26" t="inlineStr">
+        <is>
+          <t>luglio</t>
+        </is>
+      </c>
+      <c r="I2" s="26" t="inlineStr">
+        <is>
+          <t>agosto</t>
+        </is>
+      </c>
+      <c r="J2" s="26" t="inlineStr">
+        <is>
+          <t>settembre</t>
+        </is>
+      </c>
+      <c r="K2" s="26" t="inlineStr">
+        <is>
+          <t>ottobre</t>
+        </is>
+      </c>
+      <c r="L2" s="26" t="inlineStr">
+        <is>
+          <t>novembre</t>
+        </is>
+      </c>
+      <c r="M2" s="26" t="inlineStr">
+        <is>
+          <t>dicembre</t>
+        </is>
+      </c>
+      <c r="N2" s="26" t="inlineStr">
+        <is>
+          <t>TOTALE_Uscite</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="26" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="26" t="inlineStr">
+        <is>
+          <t>Acquisti convento</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7189.83</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11132.43</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10812.23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7561.69</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7236.06</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12608.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6803.33</v>
+      </c>
+      <c r="I4" t="n">
+        <v>8087.47</v>
+      </c>
+      <c r="J4" t="n">
+        <v>16440.48</v>
+      </c>
+      <c r="K4" t="n">
+        <v>36914.6</v>
+      </c>
+      <c r="L4" t="n">
+        <v>16465.63</v>
+      </c>
+      <c r="M4" t="n">
+        <v>7881.59</v>
+      </c>
+      <c r="N4" t="n">
+        <v>149133.84</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="26" t="inlineStr">
+        <is>
+          <t>Acquisti: Chiesa</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>666.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>514.4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>822.16</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1575.5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>558</v>
+      </c>
+      <c r="G5" t="n">
+        <v>423.19</v>
+      </c>
+      <c r="H5" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1220</v>
+      </c>
+      <c r="J5" t="n">
+        <v>532.55</v>
+      </c>
+      <c r="K5" t="n">
+        <v>638</v>
+      </c>
+      <c r="L5" t="n">
+        <v>511.75</v>
+      </c>
+      <c r="M5" t="n">
+        <v>643.4</v>
+      </c>
+      <c r="N5" t="n">
+        <v>8226.950000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="26" t="inlineStr">
+        <is>
+          <t>Acquisti: Orto, Animali</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5318.39</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4624.14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6540.7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12311.94</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9302.24</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2670.8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>902</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3377</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1606.66</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3510.2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4585.74</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2371.75</v>
+      </c>
+      <c r="N6" t="n">
+        <v>57121.56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="26" t="inlineStr">
+        <is>
+          <t>Cultura</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4108.22</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5224.27</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4475.29</v>
+      </c>
+      <c r="E7" t="n">
+        <v>16217.53</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5519.43</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5967.48</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1668.89</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1460.8</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4597.5</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1305.26</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4815.7</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2184.01</v>
+      </c>
+      <c r="N7" t="n">
+        <v>57544.38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="inlineStr">
+        <is>
+          <t>Curia provinciale</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12434</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9951.9</v>
+      </c>
+      <c r="E8" t="n">
+        <v>300</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3800</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>32500</v>
+      </c>
+      <c r="N8" t="n">
+        <v>68985.89999999999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="26" t="inlineStr">
+        <is>
+          <t>Domestici</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>900</v>
+      </c>
+      <c r="C9" t="n">
+        <v>900</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1051.6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>900</v>
+      </c>
+      <c r="F9" t="n">
+        <v>900</v>
+      </c>
+      <c r="G9" t="n">
+        <v>900</v>
+      </c>
+      <c r="H9" t="n">
+        <v>900</v>
+      </c>
+      <c r="I9" t="n">
+        <v>900</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1050</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3464.34</v>
+      </c>
+      <c r="M9" t="n">
+        <v>910</v>
+      </c>
+      <c r="N9" t="n">
+        <v>14575.94</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="26" t="inlineStr">
+        <is>
+          <t>Elargizioni</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9285.6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>7422</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4985</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9138.75</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4882</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3457.9</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5485.83</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6446</v>
+      </c>
+      <c r="J10" t="n">
+        <v>12321</v>
+      </c>
+      <c r="K10" t="n">
+        <v>11805.55</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2881.5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8316</v>
+      </c>
+      <c r="N10" t="n">
+        <v>86427.13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="26" t="inlineStr">
+        <is>
+          <t>Energia Elettrica</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6881.51</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10108.87</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7098.32</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7836.31</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4419.2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5830.61</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3132.44</v>
+      </c>
+      <c r="I11" t="n">
+        <v>6354.92</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4133.14</v>
+      </c>
+      <c r="K11" t="n">
+        <v>4897.45</v>
+      </c>
+      <c r="L11" t="n">
+        <v>5759.79</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5976.35</v>
+      </c>
+      <c r="N11" t="n">
+        <v>72428.91</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="26" t="inlineStr">
+        <is>
+          <t>Ferie e Viaggi</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8066.67</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4589.21</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6580.56</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6866.58</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7697</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4040.23</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4296.7</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4399.31</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5266.77</v>
+      </c>
+      <c r="K12" t="n">
+        <v>5543.1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>6795.87</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3340.15</v>
+      </c>
+      <c r="N12" t="n">
+        <v>67482.14999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="26" t="inlineStr">
+        <is>
+          <t>Igiene</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>958.08</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1646.87</v>
+      </c>
+      <c r="D13" t="n">
+        <v>431.41</v>
+      </c>
+      <c r="E13" t="n">
+        <v>473.53</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1053.95</v>
+      </c>
+      <c r="G13" t="n">
+        <v>733.6799999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>811.91</v>
+      </c>
+      <c r="I13" t="n">
+        <v>786.3200000000001</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1823.3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1078.62</v>
+      </c>
+      <c r="L13" t="n">
+        <v>903.54</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1180.98</v>
+      </c>
+      <c r="N13" t="n">
+        <v>11882.19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="26" t="inlineStr">
+        <is>
+          <t>Imposte</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2486.27</v>
+      </c>
+      <c r="C14" t="n">
+        <v>292.27</v>
+      </c>
+      <c r="D14" t="n">
+        <v>96.23</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1141.86</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1243.42</v>
+      </c>
+      <c r="G14" t="n">
+        <v>779.17</v>
+      </c>
+      <c r="H14" t="n">
+        <v>824.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>227.4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2331.03</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1165.19</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1501.65</v>
+      </c>
+      <c r="N14" t="n">
+        <v>13097.69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="26" t="inlineStr">
+        <is>
+          <t>Lavori e Impianti</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>14150</v>
+      </c>
+      <c r="C15" t="n">
+        <v>25997</v>
+      </c>
+      <c r="D15" t="n">
+        <v>35216.62</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35690</v>
+      </c>
+      <c r="F15" t="n">
+        <v>34755.24</v>
+      </c>
+      <c r="G15" t="n">
+        <v>24462.74</v>
+      </c>
+      <c r="H15" t="n">
+        <v>9150</v>
+      </c>
+      <c r="I15" t="n">
+        <v>13130</v>
+      </c>
+      <c r="J15" t="n">
+        <v>17796</v>
+      </c>
+      <c r="K15" t="n">
+        <v>830</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2520</v>
+      </c>
+      <c r="M15" t="n">
+        <v>41650</v>
+      </c>
+      <c r="N15" t="n">
+        <v>255347.6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="26" t="inlineStr">
+        <is>
+          <t>Posta e Cancelleria</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="26" t="inlineStr">
+        <is>
+          <t>Posta e cancelleria</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>237</v>
+      </c>
+      <c r="C17" t="n">
+        <v>463.06</v>
+      </c>
+      <c r="D17" t="n">
+        <v>538.02</v>
+      </c>
+      <c r="E17" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="F17" t="n">
+        <v>257.15</v>
+      </c>
+      <c r="G17" t="n">
+        <v>204.5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>181.2</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1170.3</v>
+      </c>
+      <c r="J17" t="n">
+        <v>968.8</v>
+      </c>
+      <c r="K17" t="n">
+        <v>132.6</v>
+      </c>
+      <c r="L17" t="n">
+        <v>367.62</v>
+      </c>
+      <c r="M17" t="n">
+        <v>508.33</v>
+      </c>
+      <c r="N17" t="n">
+        <v>5569.92</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="26" t="inlineStr">
+        <is>
+          <t>Rimborsi</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>34641.83</v>
+      </c>
+      <c r="C18" t="n">
+        <v>22531.9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3651.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>29294.95</v>
+      </c>
+      <c r="F18" t="n">
+        <v>15202.6</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23672.69</v>
+      </c>
+      <c r="H18" t="n">
+        <v>9779.950000000001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>20813.73</v>
+      </c>
+      <c r="J18" t="n">
+        <v>17228.75</v>
+      </c>
+      <c r="K18" t="n">
+        <v>23562.94</v>
+      </c>
+      <c r="L18" t="n">
+        <v>20955.54</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2347.94</v>
+      </c>
+      <c r="N18" t="n">
+        <v>223684.32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="26" t="inlineStr">
+        <is>
+          <t>Riscaldamento</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>14559.79</v>
+      </c>
+      <c r="C19" t="n">
+        <v>648</v>
+      </c>
+      <c r="D19" t="n">
+        <v>18471.51</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8488.77</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5055.31</v>
+      </c>
+      <c r="G19" t="n">
+        <v>484.93</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2495.29</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1744.5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>9767.200000000001</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6262.89</v>
+      </c>
+      <c r="M19" t="n">
+        <v>648.99</v>
+      </c>
+      <c r="N19" t="n">
+        <v>68627.17999999999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="26" t="inlineStr">
+        <is>
+          <t>Telefono</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>441.22</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2741.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2649.78</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3109</v>
+      </c>
+      <c r="F20" t="n">
+        <v>160</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2497.72</v>
+      </c>
+      <c r="H20" t="n">
+        <v>30</v>
+      </c>
+      <c r="I20" t="n">
+        <v>3637.22</v>
+      </c>
+      <c r="J20" t="n">
+        <v>811.0700000000001</v>
+      </c>
+      <c r="K20" t="n">
+        <v>2235.5</v>
+      </c>
+      <c r="L20" t="n">
+        <v>238.57</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2080.5</v>
+      </c>
+      <c r="N20" t="n">
+        <v>20632.08</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="26" t="inlineStr">
+        <is>
+          <t>Veicoli a Motore</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1174</v>
+      </c>
+      <c r="C21" t="n">
+        <v>497</v>
+      </c>
+      <c r="D21" t="n">
+        <v>936</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1482.28</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>4089.28</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="26" t="inlineStr">
+        <is>
+          <t>Veicoli a motore</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>7951.44</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2467.25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2168.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2133</v>
+      </c>
+      <c r="F22" t="n">
+        <v>6192.43</v>
+      </c>
+      <c r="G22" t="n">
+        <v>6581.5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>10157.94</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3540</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3978.62</v>
+      </c>
+      <c r="K22" t="n">
+        <v>17929.68</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10520.3</v>
+      </c>
+      <c r="M22" t="n">
+        <v>23721.92</v>
+      </c>
+      <c r="N22" t="n">
+        <v>97342.58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="26" t="inlineStr">
+        <is>
+          <t>Vestiario</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>483.3</v>
+      </c>
+      <c r="C23" t="n">
+        <v>883.5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>409.17</v>
+      </c>
+      <c r="E23" t="n">
+        <v>536.55</v>
+      </c>
+      <c r="F23" t="n">
+        <v>529.1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1082.38</v>
+      </c>
+      <c r="H23" t="n">
+        <v>300.8</v>
+      </c>
+      <c r="I23" t="n">
+        <v>412.4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1475</v>
+      </c>
+      <c r="K23" t="n">
+        <v>218.7</v>
+      </c>
+      <c r="L23" t="n">
+        <v>540.4</v>
+      </c>
+      <c r="M23" t="n">
+        <v>256.7</v>
+      </c>
+      <c r="N23" t="n">
+        <v>7128</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="26" t="inlineStr">
+        <is>
+          <t>Vitto</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>12753.51</v>
+      </c>
+      <c r="C24" t="n">
+        <v>12962.27</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16998.18</v>
+      </c>
+      <c r="E24" t="n">
+        <v>14145.17</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11332.16</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9092.51</v>
+      </c>
+      <c r="H24" t="n">
+        <v>8280.43</v>
+      </c>
+      <c r="I24" t="n">
+        <v>13413.55</v>
+      </c>
+      <c r="J24" t="n">
+        <v>12303.48</v>
+      </c>
+      <c r="K24" t="n">
+        <v>10119.62</v>
+      </c>
+      <c r="L24" t="n">
+        <v>9472.049999999999</v>
+      </c>
+      <c r="M24" t="n">
+        <v>13276.56</v>
+      </c>
+      <c r="N24" t="n">
+        <v>144149.49</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="26" t="inlineStr">
+        <is>
+          <t>TOTALE_Uscite</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>144689.16</v>
+      </c>
+      <c r="C25" t="n">
+        <v>125645.94</v>
+      </c>
+      <c r="D25" t="n">
+        <v>133884.68</v>
+      </c>
+      <c r="E25" t="n">
+        <v>159744.75</v>
+      </c>
+      <c r="F25" t="n">
+        <v>116295.29</v>
+      </c>
+      <c r="G25" t="n">
+        <v>105490.53</v>
+      </c>
+      <c r="H25" t="n">
+        <v>62827.42</v>
+      </c>
+      <c r="I25" t="n">
+        <v>95671.71000000001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>106408.65</v>
+      </c>
+      <c r="K25" t="n">
+        <v>133297.72</v>
+      </c>
+      <c r="L25" t="n">
+        <v>98226.42</v>
+      </c>
+      <c r="M25" t="n">
+        <v>151296.82</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1433479.09</v>
       </c>
     </row>
   </sheetData>
@@ -10317,264 +12145,264 @@
   </cols>
   <sheetData>
     <row r="1" ht="100" customHeight="1">
-      <c r="A1" s="26" t="inlineStr">
+      <c r="A1" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Tabella Entrate - Uscite - Saldo di ogni mese </t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27" t="inlineStr">
+      <c r="A2" s="28" t="inlineStr">
         <is>
           <t>mese</t>
         </is>
       </c>
-      <c r="B2" s="28" t="inlineStr">
+      <c r="B2" s="29" t="inlineStr">
         <is>
           <t>saldo_iniziale</t>
         </is>
       </c>
-      <c r="C2" s="28" t="inlineStr">
+      <c r="C2" s="29" t="inlineStr">
         <is>
           <t>entrate_mese</t>
         </is>
       </c>
-      <c r="D2" s="28" t="inlineStr">
+      <c r="D2" s="29" t="inlineStr">
         <is>
           <t>uscite_mese</t>
         </is>
       </c>
-      <c r="E2" s="28" t="inlineStr">
+      <c r="E2" s="29" t="inlineStr">
         <is>
           <t>saldo_finale</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="28" t="inlineStr">
+      <c r="A3" s="29" t="inlineStr">
         <is>
           <t>gennaio</t>
         </is>
       </c>
-      <c r="B3" s="29" t="n">
+      <c r="B3" s="30" t="n">
         <v>200000</v>
       </c>
-      <c r="C3" s="30" t="n">
+      <c r="C3" s="31" t="n">
         <v>102266.604</v>
       </c>
-      <c r="D3" s="30" t="n">
+      <c r="D3" s="31" t="n">
         <v>144689.16</v>
       </c>
-      <c r="E3" s="30" t="n">
+      <c r="E3" s="31" t="n">
         <v>157577.444</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="28" t="inlineStr">
+      <c r="A4" s="29" t="inlineStr">
         <is>
           <t>febbraio</t>
         </is>
       </c>
-      <c r="B4" s="30" t="n">
+      <c r="B4" s="31" t="n">
         <v>157577.444</v>
       </c>
-      <c r="C4" s="30" t="n">
+      <c r="C4" s="31" t="n">
         <v>77543.88</v>
       </c>
-      <c r="D4" s="30" t="n">
+      <c r="D4" s="31" t="n">
         <v>125645.94</v>
       </c>
-      <c r="E4" s="30" t="n">
+      <c r="E4" s="31" t="n">
         <v>115154.888</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="28" t="inlineStr">
+      <c r="A5" s="29" t="inlineStr">
         <is>
           <t>marzo</t>
         </is>
       </c>
-      <c r="B5" s="30" t="n">
+      <c r="B5" s="31" t="n">
         <v>115154.888</v>
       </c>
-      <c r="C5" s="30" t="n">
+      <c r="C5" s="31" t="n">
         <v>77550.48999999999</v>
       </c>
-      <c r="D5" s="30" t="n">
+      <c r="D5" s="31" t="n">
         <v>133884.68</v>
       </c>
-      <c r="E5" s="30" t="n">
+      <c r="E5" s="31" t="n">
         <v>72732.33199999997</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="28" t="inlineStr">
+      <c r="A6" s="29" t="inlineStr">
         <is>
           <t>aprile</t>
         </is>
       </c>
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="31" t="n">
         <v>72732.33199999997</v>
       </c>
-      <c r="C6" s="30" t="n">
+      <c r="C6" s="31" t="n">
         <v>100705.39</v>
       </c>
-      <c r="D6" s="30" t="n">
+      <c r="D6" s="31" t="n">
         <v>159744.75</v>
       </c>
-      <c r="E6" s="30" t="n">
+      <c r="E6" s="31" t="n">
         <v>30309.77599999995</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="28" t="inlineStr">
+      <c r="A7" s="29" t="inlineStr">
         <is>
           <t>maggio</t>
         </is>
       </c>
-      <c r="B7" s="30" t="n">
+      <c r="B7" s="31" t="n">
         <v>30309.77599999995</v>
       </c>
-      <c r="C7" s="30" t="n">
+      <c r="C7" s="31" t="n">
         <v>107413.59</v>
       </c>
-      <c r="D7" s="30" t="n">
+      <c r="D7" s="31" t="n">
         <v>116295.29</v>
       </c>
-      <c r="E7" s="31" t="n">
+      <c r="E7" s="32" t="n">
         <v>-12112.78000000006</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="28" t="inlineStr">
+      <c r="A8" s="29" t="inlineStr">
         <is>
           <t>giugno</t>
         </is>
       </c>
-      <c r="B8" s="31" t="n">
+      <c r="B8" s="32" t="n">
         <v>-12112.78000000006</v>
       </c>
-      <c r="C8" s="30" t="n">
+      <c r="C8" s="31" t="n">
         <v>58442.47</v>
       </c>
-      <c r="D8" s="30" t="n">
+      <c r="D8" s="31" t="n">
         <v>105490.53</v>
       </c>
-      <c r="E8" s="31" t="n">
+      <c r="E8" s="32" t="n">
         <v>-54535.33600000007</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="28" t="inlineStr">
+      <c r="A9" s="29" t="inlineStr">
         <is>
           <t>luglio</t>
         </is>
       </c>
-      <c r="B9" s="31" t="n">
+      <c r="B9" s="32" t="n">
         <v>-54535.33600000007</v>
       </c>
-      <c r="C9" s="30" t="n">
+      <c r="C9" s="31" t="n">
         <v>59532.41</v>
       </c>
-      <c r="D9" s="30" t="n">
+      <c r="D9" s="31" t="n">
         <v>62827.42</v>
       </c>
-      <c r="E9" s="31" t="n">
+      <c r="E9" s="32" t="n">
         <v>-96957.89200000008</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="28" t="inlineStr">
+      <c r="A10" s="29" t="inlineStr">
         <is>
           <t>agosto</t>
         </is>
       </c>
-      <c r="B10" s="31" t="n">
+      <c r="B10" s="32" t="n">
         <v>-96957.89200000008</v>
       </c>
-      <c r="C10" s="30" t="n">
+      <c r="C10" s="31" t="n">
         <v>66470.95</v>
       </c>
-      <c r="D10" s="30" t="n">
+      <c r="D10" s="31" t="n">
         <v>95671.71000000002</v>
       </c>
-      <c r="E10" s="31" t="n">
+      <c r="E10" s="32" t="n">
         <v>-139380.4480000001</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="28" t="inlineStr">
+      <c r="A11" s="29" t="inlineStr">
         <is>
           <t>settembre</t>
         </is>
       </c>
-      <c r="B11" s="31" t="n">
+      <c r="B11" s="32" t="n">
         <v>-139380.4480000001</v>
       </c>
-      <c r="C11" s="30" t="n">
+      <c r="C11" s="31" t="n">
         <v>78144.25999999999</v>
       </c>
-      <c r="D11" s="30" t="n">
+      <c r="D11" s="31" t="n">
         <v>106408.65</v>
       </c>
-      <c r="E11" s="31" t="n">
+      <c r="E11" s="32" t="n">
         <v>-181803.0040000001</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="28" t="inlineStr">
+      <c r="A12" s="29" t="inlineStr">
         <is>
           <t>ottobre</t>
         </is>
       </c>
-      <c r="B12" s="31" t="n">
+      <c r="B12" s="32" t="n">
         <v>-181803.0040000001</v>
       </c>
-      <c r="C12" s="30" t="n">
+      <c r="C12" s="31" t="n">
         <v>97706.60000000001</v>
       </c>
-      <c r="D12" s="30" t="n">
+      <c r="D12" s="31" t="n">
         <v>133297.72</v>
       </c>
-      <c r="E12" s="31" t="n">
+      <c r="E12" s="32" t="n">
         <v>-224225.5600000001</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="28" t="inlineStr">
+      <c r="A13" s="29" t="inlineStr">
         <is>
           <t>novembre</t>
         </is>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="32" t="n">
         <v>-224225.5600000001</v>
       </c>
-      <c r="C13" s="30" t="n">
+      <c r="C13" s="31" t="n">
         <v>70497.86</v>
       </c>
-      <c r="D13" s="30" t="n">
+      <c r="D13" s="31" t="n">
         <v>98226.42000000001</v>
       </c>
-      <c r="E13" s="31" t="n">
+      <c r="E13" s="32" t="n">
         <v>-266648.1160000002</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="28" t="inlineStr">
+      <c r="A14" s="29" t="inlineStr">
         <is>
           <t>dicembre</t>
         </is>
       </c>
-      <c r="B14" s="31" t="n">
+      <c r="B14" s="32" t="n">
         <v>-266648.1160000002</v>
       </c>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="31" t="n">
         <v>102393.39</v>
       </c>
-      <c r="D14" s="30" t="n">
+      <c r="D14" s="31" t="n">
         <v>151296.82</v>
       </c>
-      <c r="E14" s="32" t="n">
+      <c r="E14" s="33" t="n">
         <v>-309070.6720000001</v>
       </c>
     </row>

</xml_diff>